<commit_message>
Added the base calculation of the Animation, Modeling and Other Services espesially Floor Plan and dollhouse. Fixed issue with not showing the hours and hourly rate fields when choosing people adding service. Made input validation by writing the function which is using with animation seconds input and people custom hourly rate
</commit_message>
<xml_diff>
--- a/data/Prices.xlsx
+++ b/data/Prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>SOW_Name</t>
   </si>
@@ -73,7 +73,7 @@
     <t>Installation Animation</t>
   </si>
   <si>
-    <t>Architectural Animation (from 10sec)</t>
+    <t>Architectural Animation</t>
   </si>
   <si>
     <t>Simple Modeling</t>
@@ -88,16 +88,16 @@
     <t>Ultra Complex Modeling</t>
   </si>
   <si>
-    <t>AR Simple Modeling</t>
-  </si>
-  <si>
-    <t>AR Medium Modeling</t>
-  </si>
-  <si>
-    <t>AR Complex Modeling</t>
-  </si>
-  <si>
-    <t>AR Ultra Complex Modeling</t>
+    <t>Simple AR Modeling</t>
+  </si>
+  <si>
+    <t>Medium AR Modeling</t>
+  </si>
+  <si>
+    <t>Complex AR Modeling</t>
+  </si>
+  <si>
+    <t>Ultra Complex AR Modeling</t>
   </si>
   <si>
     <t>Simple Texture/Material Creation</t>
@@ -106,13 +106,13 @@
     <t>Complex Texture/Material Creation</t>
   </si>
   <si>
-    <t xml:space="preserve">Silo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">360 view (60 images) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simple Indoor Lifestyle </t>
+    <t>Silo</t>
+  </si>
+  <si>
+    <t>360 view (60 images)</t>
+  </si>
+  <si>
+    <t>Simple Indoor Lifestyle</t>
   </si>
   <si>
     <t>Medium Indoor Lifestyle</t>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Complex Outdoor Lifestyle</t>
+  </si>
+  <si>
+    <t>Template Lifestyle</t>
   </si>
   <si>
     <t>1-2 people</t>
@@ -176,37 +179,19 @@
     <t>Additional render (existing space)</t>
   </si>
   <si>
-    <t>SOW</t>
-  </si>
-  <si>
-    <t>Revit Model</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ratio Change </t>
   </si>
   <si>
-    <t>Technical Quality</t>
-  </si>
-  <si>
     <t xml:space="preserve">Zoom In </t>
   </si>
   <si>
-    <t xml:space="preserve">Design     </t>
-  </si>
-  <si>
     <t xml:space="preserve">Zoom out (up to 20%) </t>
   </si>
   <si>
     <t xml:space="preserve">Opposite elevation </t>
   </si>
   <si>
-    <t>Revisions</t>
-  </si>
-  <si>
     <t xml:space="preserve">Side elevation </t>
-  </si>
-  <si>
-    <t>Extra 1 round</t>
   </si>
   <si>
     <t>Additional
@@ -216,13 +201,7 @@
     <t xml:space="preserve">Props </t>
   </si>
   <si>
-    <t>Extra 2 round</t>
-  </si>
-  <si>
     <t xml:space="preserve">Colors </t>
-  </si>
-  <si>
-    <t>Extra 3 round</t>
   </si>
   <si>
     <t xml:space="preserve">Finishes </t>
@@ -380,6 +359,17 @@
       </bottom>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -446,17 +436,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -476,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -497,6 +476,9 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -504,18 +486,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -524,33 +518,33 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="7" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="2" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="2" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -931,7 +925,7 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="4">
@@ -971,7 +965,7 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="4">
@@ -979,7 +973,7 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="4">
@@ -987,7 +981,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="4">
@@ -995,7 +989,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="4">
@@ -1003,10 +997,10 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="10">
         <v>30.0</v>
       </c>
     </row>
@@ -1019,34 +1013,34 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="10">
         <v>30.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="10">
         <v>100.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="10">
         <v>300.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="10">
         <v>400.0</v>
       </c>
     </row>
@@ -1083,45 +1077,45 @@
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="13">
+        <v>240.0</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4">
         <v>90.0</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="4">
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="4">
         <v>160.0</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="4">
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4">
         <v>310.0</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="4">
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="4">
         <v>20.0</v>
       </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="4">
-        <v>500.0</v>
-      </c>
-      <c r="F40" s="12"/>
+      <c r="F40" s="16"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -1129,113 +1123,120 @@
         <v>41</v>
       </c>
       <c r="B41" s="4">
-        <v>1400.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="4">
-        <v>600.0</v>
+      <c r="B42" s="17">
+        <v>500.0</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="4">
-        <v>1600.0</v>
+      <c r="B43" s="17">
+        <v>1400.0</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="4">
-        <v>100.0</v>
+      <c r="B44" s="17">
+        <v>600.0</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="4">
-        <v>200.0</v>
-      </c>
-      <c r="C45" s="13"/>
+      <c r="B45" s="17">
+        <v>1600.0</v>
+      </c>
+      <c r="C45" s="18"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="4">
-        <v>40.0</v>
-      </c>
-      <c r="C46" s="13"/>
+        <v>200.0</v>
+      </c>
+      <c r="C46" s="18"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="4">
-        <v>20.0</v>
-      </c>
-      <c r="C47" s="13"/>
+        <v>40.0</v>
+      </c>
+      <c r="C47" s="18"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="14">
+      <c r="B48" s="4">
         <v>20.0</v>
       </c>
     </row>
-    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="19">
+        <v>20.0</v>
+      </c>
+    </row>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="13"/>
+      <c r="C55" s="18"/>
     </row>
     <row r="56" ht="15.75" customHeight="1"/>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1"/>
     <row r="59" ht="15.75" customHeight="1"/>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="13"/>
+      <c r="C60" s="18"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="15"/>
+      <c r="C61" s="20"/>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="15"/>
+      <c r="C65" s="20"/>
     </row>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="16"/>
+      <c r="C69" s="21"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="13"/>
+      <c r="C70" s="18"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="16"/>
+      <c r="C71" s="21"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="16"/>
+      <c r="C72" s="21"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="16"/>
+      <c r="C73" s="21"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="15"/>
+      <c r="C74" s="20"/>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>
     <row r="76" ht="15.75" customHeight="1"/>
@@ -2165,13 +2166,13 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="C47:C54"/>
+    <mergeCell ref="C55:C59"/>
+    <mergeCell ref="C60:E60"/>
     <mergeCell ref="C61:C64"/>
-    <mergeCell ref="C55:C59"/>
     <mergeCell ref="C65:C68"/>
     <mergeCell ref="C74:C81"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C47:C54"/>
-    <mergeCell ref="E16:E20"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2188,173 +2189,145 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="19">
+      <c r="B1" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="24">
         <v>0.24</v>
       </c>
-      <c r="E1" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="22">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="24">
+        <v>0.24</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C3" s="24">
         <v>0.24</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="6" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="28"/>
+      <c r="B4" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="26">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24" t="s">
+      <c r="C4" s="24">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="28"/>
+      <c r="B5" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="19">
-        <v>0.24</v>
-      </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28" t="s">
+      <c r="C5" s="24">
+        <v>0.64</v>
+      </c>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="37"/>
+      <c r="B6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="29">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="23"/>
-      <c r="B4" s="18" t="s">
+      <c r="C6" s="24">
+        <v>0.34</v>
+      </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="39"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="19">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="23"/>
-      <c r="B5" s="18" t="s">
+      <c r="B7" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="19">
-        <v>0.64</v>
-      </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="31" t="s">
+      <c r="C7" s="24">
+        <v>0.22</v>
+      </c>
+      <c r="F7" s="38"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="39"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="28"/>
+      <c r="B8" s="23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="32"/>
-      <c r="B6" s="24" t="s">
+      <c r="C8" s="24">
+        <v>0.22</v>
+      </c>
+      <c r="F8" s="38"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="39"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="19">
-        <v>0.34</v>
-      </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="31" t="s">
+      <c r="C9" s="24">
+        <v>0.22</v>
+      </c>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="34">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="17" t="s">
+      <c r="C10" s="24">
+        <v>0.31</v>
+      </c>
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="28"/>
+      <c r="B11" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C11" s="24">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="28"/>
+      <c r="B12" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="19">
-        <v>0.22</v>
-      </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="31" t="s">
+      <c r="C12" s="24">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="37"/>
+      <c r="B13" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="34">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="23"/>
-      <c r="B8" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="19">
-        <v>0.22</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="34">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="19">
-        <v>0.22</v>
-      </c>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="19">
-        <v>0.31</v>
-      </c>
-      <c r="F10" s="33"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="23"/>
-      <c r="B11" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="19">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="23"/>
-      <c r="B12" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="19">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="32"/>
-      <c r="B13" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="19">
+      <c r="C13" s="24">
         <v>0.45</v>
       </c>
     </row>
@@ -2382,129 +2355,129 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="42">
+        <v>109.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="42">
+        <v>69.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="42">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="42">
+        <v>420.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="42">
+        <v>999.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B7" s="42">
+        <v>3299.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="43" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="36" t="s">
+      <c r="B8" s="42">
+        <v>645.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="37">
-        <v>109.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="38" t="s">
+      <c r="B9" s="42">
+        <v>325.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="37">
-        <v>69.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="38" t="s">
+      <c r="B10" s="42">
+        <v>228.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="37">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="38" t="s">
+      <c r="B11" s="42">
+        <v>230.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="37">
-        <v>420.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="38" t="s">
+      <c r="B12" s="42">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="37">
-        <v>999.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="38" t="s">
+      <c r="B13" s="42">
+        <v>79.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="37">
-        <v>3299.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="38" t="s">
+      <c r="B14" s="42">
+        <v>198.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="37">
-        <v>645.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="38" t="s">
+      <c r="B15" s="42">
+        <v>795.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="37">
-        <v>325.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="37">
-        <v>228.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="37">
-        <v>230.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="37">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="37">
-        <v>79.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="37">
-        <v>198.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="37">
-        <v>795.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="37">
+      <c r="B16" s="42">
         <v>295.0</v>
       </c>
     </row>

</xml_diff>